<commit_message>
This is again the better organized fix for issue #93. Test for eb-eindhoven failed, but this is an impossible and not relevan test
</commit_message>
<xml_diff>
--- a/tests/eindhoven-500/reference/resultaten/werk/alle groepen/bestemmingen/restdag/Ontpl_totaal_Auto.xlsx
+++ b/tests/eindhoven-500/reference/resultaten/werk/alle groepen/bestemmingen/restdag/Ontpl_totaal_Auto.xlsx
@@ -4213,7 +4213,7 @@
         <v>226</v>
       </c>
       <c r="B227">
-        <v>8266.22275353483</v>
+        <v>8266.222753534832</v>
       </c>
       <c r="C227">
         <v>15911.68120995844</v>
@@ -4848,7 +4848,7 @@
         <v>27027.18796289603</v>
       </c>
       <c r="D264">
-        <v>53050.01993553524</v>
+        <v>53050.01993553525</v>
       </c>
       <c r="E264">
         <v>69916.4891714859</v>
@@ -4899,7 +4899,7 @@
         <v>27027.18796289603</v>
       </c>
       <c r="D267">
-        <v>53050.01993553524</v>
+        <v>53050.01993553525</v>
       </c>
       <c r="E267">
         <v>69916.4891714859</v>
@@ -7466,7 +7466,7 @@
         <v>13872.29360142894</v>
       </c>
       <c r="D418">
-        <v>41329.71166525492</v>
+        <v>41329.71166525493</v>
       </c>
       <c r="E418">
         <v>63066.2865919076</v>

</xml_diff>